<commit_message>
test case 01 complete
commit 6
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataFile.xlsx
+++ b/src/main/resources/Data/DataFile.xlsx
@@ -9,11 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TC01_Login" sheetId="1" r:id="rId1"/>
+    <sheet name="TC02_RegisterAccount" sheetId="2" r:id="rId2"/>
+    <sheet name="Resources" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="listcountry">Resources!$A$2:$A$3</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -21,6 +26,35 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>user300@gmail.com</t>
+  </si>
+  <si>
+    <t>123456789oO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Name </t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>List countries</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +373,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>listcountry</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>